<commit_message>
adding short cycling ratio var
</commit_message>
<xml_diff>
--- a/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
+++ b/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdahlhau\Documents\GitHub\NREL\comstock\measures\comstock_sensitivity_reports\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkim4\Documents\GitHub\ComStock\measures\comstock_sensitivity_reports\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95747AC8-956C-46FC-85F3-4170987305CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D5FB5D-3D5E-47DD-8948-C310BBB7A524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="-4620" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="945">
   <si>
     <t>Input List</t>
   </si>
@@ -2863,6 +2863,18 @@
   </si>
   <si>
     <t>com_report_hvac_vrf_heating_design_cop_minus_22_f</t>
+  </si>
+  <si>
+    <t>Heat pump heating cycling ratio weighted by heating rate</t>
+  </si>
+  <si>
+    <t>com_report_hvac_heat_pump_heating_cycling_ratio</t>
+  </si>
+  <si>
+    <t>Heat pump cooling cycling ratio weighted by cooling rate</t>
+  </si>
+  <si>
+    <t>com_report_hvac_heat_pump_cooling_cycling_ratio</t>
   </si>
 </sst>
 </file>
@@ -3020,9 +3032,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3060,7 +3072,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3166,7 +3178,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3308,7 +3320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3322,16 +3334,16 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3351,7 +3363,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3368,7 +3380,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3382,7 +3394,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3396,7 +3408,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -3410,7 +3422,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3424,7 +3436,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3438,7 +3450,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3452,7 +3464,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3466,7 +3478,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3480,7 +3492,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -3494,7 +3506,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3511,7 +3523,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -3525,7 +3537,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3539,7 +3551,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3553,7 +3565,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -3570,7 +3582,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3584,7 +3596,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3598,7 +3610,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3612,7 +3624,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3626,7 +3638,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3643,7 +3655,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -3657,7 +3669,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>112</v>
       </c>
@@ -3674,7 +3686,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3691,7 +3703,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -3705,7 +3717,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3722,7 +3734,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3739,7 +3751,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -3753,7 +3765,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -3767,7 +3779,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3784,7 +3796,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3798,7 +3810,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3815,7 +3827,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -3829,7 +3841,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3846,7 +3858,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -3860,7 +3872,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3874,7 +3886,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -3891,7 +3903,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -3905,7 +3917,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3919,7 +3931,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3933,7 +3945,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -3947,7 +3959,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -3961,7 +3973,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -3975,7 +3987,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -3989,7 +4001,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -4006,7 +4018,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>108</v>
       </c>
@@ -4020,7 +4032,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4037,7 +4049,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -4051,7 +4063,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -4065,7 +4077,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -4079,7 +4091,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -4096,7 +4108,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4110,7 +4122,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -4124,7 +4136,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -4138,7 +4150,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -4152,7 +4164,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4169,7 +4181,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -4183,7 +4195,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -4197,7 +4209,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -4211,7 +4223,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -4225,7 +4237,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -4239,7 +4251,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -4253,7 +4265,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -4267,7 +4279,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -4281,7 +4293,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -4295,7 +4307,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -4309,7 +4321,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -4326,7 +4338,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -4340,7 +4352,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4354,7 +4366,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -4371,7 +4383,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -4385,7 +4397,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -4399,7 +4411,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -4413,7 +4425,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -4430,7 +4442,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -4447,7 +4459,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -4461,7 +4473,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -4475,7 +4487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -4489,7 +4501,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -4503,7 +4515,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -4517,7 +4529,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -4531,7 +4543,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -4545,7 +4557,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4559,7 +4571,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -4576,7 +4588,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -4621,7 +4633,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -4635,7 +4647,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -4652,7 +4664,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>133</v>
       </c>
@@ -4677,28 +4689,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE568D5-2279-4922-8B77-550F2E5B90B6}">
-  <dimension ref="A1:K334"/>
+  <dimension ref="A1:K336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="102" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>176</v>
       </c>
@@ -4733,7 +4746,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>525</v>
       </c>
@@ -4759,7 +4772,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>526</v>
       </c>
@@ -4785,7 +4798,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>523</v>
       </c>
@@ -4811,7 +4824,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>524</v>
       </c>
@@ -4837,7 +4850,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>533</v>
       </c>
@@ -4863,7 +4876,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>453</v>
       </c>
@@ -4889,7 +4902,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>455</v>
       </c>
@@ -4915,7 +4928,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>454</v>
       </c>
@@ -4941,7 +4954,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>534</v>
       </c>
@@ -4967,7 +4980,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>452</v>
       </c>
@@ -4993,7 +5006,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -5016,7 +5029,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -5045,7 +5058,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>254</v>
       </c>
@@ -5065,7 +5078,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>255</v>
       </c>
@@ -5085,7 +5098,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>936</v>
       </c>
@@ -5111,7 +5124,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>938</v>
       </c>
@@ -5137,7 +5150,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>939</v>
       </c>
@@ -5163,7 +5176,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>937</v>
       </c>
@@ -5189,7 +5202,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -5215,7 +5228,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -5241,7 +5254,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -5267,7 +5280,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>475</v>
       </c>
@@ -5293,7 +5306,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>207</v>
       </c>
@@ -5322,7 +5335,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>472</v>
       </c>
@@ -5348,7 +5361,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>479</v>
       </c>
@@ -5374,7 +5387,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -5400,7 +5413,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -5426,7 +5439,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -5452,7 +5465,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -5478,7 +5491,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -5501,7 +5514,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -5524,7 +5537,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -5547,7 +5560,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>162</v>
       </c>
@@ -5570,7 +5583,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -5596,7 +5609,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -5616,7 +5629,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -5636,7 +5649,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -5656,7 +5669,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -5676,7 +5689,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -5696,7 +5709,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -5716,7 +5729,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -5736,7 +5749,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -5756,7 +5769,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -5776,7 +5789,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -5796,7 +5809,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>266</v>
       </c>
@@ -5822,7 +5835,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>268</v>
       </c>
@@ -5848,7 +5861,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>267</v>
       </c>
@@ -5874,7 +5887,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>230</v>
       </c>
@@ -5900,7 +5913,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>231</v>
       </c>
@@ -5926,7 +5939,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>233</v>
       </c>
@@ -5952,7 +5965,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>232</v>
       </c>
@@ -5978,7 +5991,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>199</v>
       </c>
@@ -6004,7 +6017,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -6031,7 +6044,7 @@
       </c>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>206</v>
       </c>
@@ -6058,7 +6071,7 @@
       </c>
       <c r="K55" s="3"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>265</v>
       </c>
@@ -6084,7 +6097,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>777</v>
       </c>
@@ -6110,7 +6123,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>781</v>
       </c>
@@ -6136,7 +6149,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>776</v>
       </c>
@@ -6162,7 +6175,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>775</v>
       </c>
@@ -6188,7 +6201,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>388</v>
       </c>
@@ -6214,7 +6227,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>393</v>
       </c>
@@ -6240,7 +6253,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>394</v>
       </c>
@@ -6266,7 +6279,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>389</v>
       </c>
@@ -6292,7 +6305,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>390</v>
       </c>
@@ -6318,7 +6331,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>391</v>
       </c>
@@ -6344,7 +6357,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>392</v>
       </c>
@@ -6370,7 +6383,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>729</v>
       </c>
@@ -6396,7 +6409,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>730</v>
       </c>
@@ -6422,7 +6435,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>733</v>
       </c>
@@ -6448,7 +6461,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>731</v>
       </c>
@@ -6474,7 +6487,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>732</v>
       </c>
@@ -6500,7 +6513,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>735</v>
       </c>
@@ -6526,7 +6539,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>734</v>
       </c>
@@ -6552,7 +6565,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>737</v>
       </c>
@@ -6578,7 +6591,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>738</v>
       </c>
@@ -6604,7 +6617,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>736</v>
       </c>
@@ -6630,7 +6643,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>741</v>
       </c>
@@ -6656,7 +6669,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>739</v>
       </c>
@@ -6682,7 +6695,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>740</v>
       </c>
@@ -6708,7 +6721,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>742</v>
       </c>
@@ -6734,7 +6747,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>743</v>
       </c>
@@ -6760,7 +6773,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>744</v>
       </c>
@@ -6786,7 +6799,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>916</v>
       </c>
@@ -6812,7 +6825,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>917</v>
       </c>
@@ -6838,7 +6851,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>919</v>
       </c>
@@ -6864,7 +6877,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>918</v>
       </c>
@@ -6890,7 +6903,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>920</v>
       </c>
@@ -6916,7 +6929,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>921</v>
       </c>
@@ -6942,7 +6955,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>746</v>
       </c>
@@ -6968,7 +6981,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>745</v>
       </c>
@@ -6994,7 +7007,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>752</v>
       </c>
@@ -7020,7 +7033,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>747</v>
       </c>
@@ -7046,7 +7059,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>795</v>
       </c>
@@ -7072,7 +7085,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>796</v>
       </c>
@@ -7098,7 +7111,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>797</v>
       </c>
@@ -7124,7 +7137,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>798</v>
       </c>
@@ -7150,7 +7163,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>748</v>
       </c>
@@ -7176,7 +7189,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>791</v>
       </c>
@@ -7202,7 +7215,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>792</v>
       </c>
@@ -7228,7 +7241,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>793</v>
       </c>
@@ -7254,7 +7267,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>794</v>
       </c>
@@ -7280,7 +7293,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>808</v>
       </c>
@@ -7306,7 +7319,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>274</v>
       </c>
@@ -7332,7 +7345,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>576</v>
       </c>
@@ -7358,7 +7371,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>552</v>
       </c>
@@ -7384,7 +7397,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>575</v>
       </c>
@@ -7410,7 +7423,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>574</v>
       </c>
@@ -7436,7 +7449,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>588</v>
       </c>
@@ -7462,7 +7475,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>586</v>
       </c>
@@ -7488,7 +7501,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>585</v>
       </c>
@@ -7514,7 +7527,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>587</v>
       </c>
@@ -7540,7 +7553,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>556</v>
       </c>
@@ -7566,7 +7579,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>77</v>
       </c>
@@ -7592,7 +7605,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>340</v>
       </c>
@@ -7618,7 +7631,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>483</v>
       </c>
@@ -7644,7 +7657,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>281</v>
       </c>
@@ -7670,7 +7683,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>283</v>
       </c>
@@ -7696,7 +7709,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>282</v>
       </c>
@@ -7722,7 +7735,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>276</v>
       </c>
@@ -7748,7 +7761,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -7774,7 +7787,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>279</v>
       </c>
@@ -7800,7 +7813,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>280</v>
       </c>
@@ -7826,7 +7839,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>277</v>
       </c>
@@ -7852,7 +7865,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>309</v>
       </c>
@@ -7878,7 +7891,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>313</v>
       </c>
@@ -7904,7 +7917,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>312</v>
       </c>
@@ -7930,7 +7943,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>310</v>
       </c>
@@ -7956,7 +7969,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>311</v>
       </c>
@@ -7982,7 +7995,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>314</v>
       </c>
@@ -8008,7 +8021,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>288</v>
       </c>
@@ -8037,7 +8050,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>290</v>
       </c>
@@ -8066,7 +8079,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>291</v>
       </c>
@@ -8095,7 +8108,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>289</v>
       </c>
@@ -8124,7 +8137,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>402</v>
       </c>
@@ -8153,7 +8166,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>292</v>
       </c>
@@ -8179,7 +8192,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>295</v>
       </c>
@@ -8205,7 +8218,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>296</v>
       </c>
@@ -8231,7 +8244,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>293</v>
       </c>
@@ -8257,7 +8270,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>294</v>
       </c>
@@ -8283,7 +8296,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>592</v>
       </c>
@@ -8309,7 +8322,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>591</v>
       </c>
@@ -8335,7 +8348,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>590</v>
       </c>
@@ -8361,7 +8374,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>589</v>
       </c>
@@ -8387,7 +8400,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>247</v>
       </c>
@@ -8414,7 +8427,7 @@
       </c>
       <c r="K145" s="3"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>106</v>
       </c>
@@ -8438,7 +8451,7 @@
       </c>
       <c r="K146" s="3"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>880</v>
       </c>
@@ -8465,7 +8478,7 @@
       </c>
       <c r="K147" s="3"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>883</v>
       </c>
@@ -8492,7 +8505,7 @@
       </c>
       <c r="K148" s="3"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
         <v>106</v>
       </c>
@@ -8516,7 +8529,7 @@
       </c>
       <c r="K149" s="3"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
         <v>106</v>
       </c>
@@ -8540,7 +8553,7 @@
       </c>
       <c r="K150" s="3"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>106</v>
       </c>
@@ -8564,7 +8577,7 @@
       </c>
       <c r="K151" s="3"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>881</v>
       </c>
@@ -8591,7 +8604,7 @@
       </c>
       <c r="K152" s="3"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>882</v>
       </c>
@@ -8618,7 +8631,7 @@
       </c>
       <c r="K153" s="3"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>106</v>
       </c>
@@ -8642,7 +8655,7 @@
       </c>
       <c r="K154" s="3"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>106</v>
       </c>
@@ -8666,7 +8679,7 @@
       </c>
       <c r="K155" s="3"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>273</v>
       </c>
@@ -8692,7 +8705,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>316</v>
       </c>
@@ -8718,7 +8731,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>246</v>
       </c>
@@ -8744,7 +8757,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>441</v>
       </c>
@@ -8770,7 +8783,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>443</v>
       </c>
@@ -8796,7 +8809,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>439</v>
       </c>
@@ -8822,7 +8835,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>445</v>
       </c>
@@ -8848,7 +8861,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>442</v>
       </c>
@@ -8874,7 +8887,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>444</v>
       </c>
@@ -8900,7 +8913,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>440</v>
       </c>
@@ -8926,7 +8939,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>446</v>
       </c>
@@ -8952,7 +8965,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>437</v>
       </c>
@@ -8978,7 +8991,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>438</v>
       </c>
@@ -9004,7 +9017,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>505</v>
       </c>
@@ -9030,7 +9043,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>510</v>
       </c>
@@ -9056,7 +9069,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>275</v>
       </c>
@@ -9082,7 +9095,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>345</v>
       </c>
@@ -9108,7 +9121,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>275</v>
       </c>
@@ -9134,7 +9147,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>484</v>
       </c>
@@ -9160,7 +9173,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>353</v>
       </c>
@@ -9186,7 +9199,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>354</v>
       </c>
@@ -9212,7 +9225,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>317</v>
       </c>
@@ -9238,7 +9251,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>456</v>
       </c>
@@ -9264,7 +9277,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>362</v>
       </c>
@@ -9290,7 +9303,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>487</v>
       </c>
@@ -9316,7 +9329,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>404</v>
       </c>
@@ -9342,7 +9355,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>363</v>
       </c>
@@ -9368,7 +9381,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>405</v>
       </c>
@@ -9394,7 +9407,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>364</v>
       </c>
@@ -9420,7 +9433,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>403</v>
       </c>
@@ -9446,7 +9459,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>400</v>
       </c>
@@ -9472,7 +9485,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>401</v>
       </c>
@@ -9498,7 +9511,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>512</v>
       </c>
@@ -9524,7 +9537,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>511</v>
       </c>
@@ -9550,7 +9563,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>450</v>
       </c>
@@ -9576,7 +9589,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>451</v>
       </c>
@@ -9602,7 +9615,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>369</v>
       </c>
@@ -9628,7 +9641,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>370</v>
       </c>
@@ -9654,7 +9667,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>368</v>
       </c>
@@ -9680,7 +9693,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>499</v>
       </c>
@@ -9706,7 +9719,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>583</v>
       </c>
@@ -9732,7 +9745,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>584</v>
       </c>
@@ -9758,7 +9771,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>501</v>
       </c>
@@ -9784,7 +9797,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>502</v>
       </c>
@@ -9810,7 +9823,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>500</v>
       </c>
@@ -9836,7 +9849,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>906</v>
       </c>
@@ -9862,7 +9875,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>907</v>
       </c>
@@ -9888,7 +9901,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>285</v>
       </c>
@@ -9914,7 +9927,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>830</v>
       </c>
@@ -9940,7 +9953,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>832</v>
       </c>
@@ -9966,7 +9979,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>834</v>
       </c>
@@ -9992,7 +10005,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>836</v>
       </c>
@@ -10018,7 +10031,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>838</v>
       </c>
@@ -10044,7 +10057,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>840</v>
       </c>
@@ -10070,7 +10083,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>843</v>
       </c>
@@ -10096,7 +10109,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>848</v>
       </c>
@@ -10122,7 +10135,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>815</v>
       </c>
@@ -10148,7 +10161,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>816</v>
       </c>
@@ -10174,7 +10187,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>820</v>
       </c>
@@ -10200,7 +10213,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>817</v>
       </c>
@@ -10226,7 +10239,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>818</v>
       </c>
@@ -10252,7 +10265,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>819</v>
       </c>
@@ -10278,7 +10291,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>826</v>
       </c>
@@ -10304,7 +10317,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>827</v>
       </c>
@@ -10330,7 +10343,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>829</v>
       </c>
@@ -10356,7 +10369,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>828</v>
       </c>
@@ -10382,7 +10395,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>849</v>
       </c>
@@ -10408,7 +10421,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>901</v>
       </c>
@@ -10434,7 +10447,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>902</v>
       </c>
@@ -10460,7 +10473,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>903</v>
       </c>
@@ -10486,7 +10499,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>857</v>
       </c>
@@ -10512,7 +10525,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>858</v>
       </c>
@@ -10538,7 +10551,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>859</v>
       </c>
@@ -10564,7 +10577,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>860</v>
       </c>
@@ -10590,7 +10603,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>861</v>
       </c>
@@ -10616,7 +10629,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>341</v>
       </c>
@@ -10642,7 +10655,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>561</v>
       </c>
@@ -10668,7 +10681,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>562</v>
       </c>
@@ -10694,7 +10707,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>560</v>
       </c>
@@ -10720,7 +10733,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>468</v>
       </c>
@@ -10746,7 +10759,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>469</v>
       </c>
@@ -10772,7 +10785,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>470</v>
       </c>
@@ -10798,7 +10811,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>471</v>
       </c>
@@ -10824,7 +10837,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>619</v>
       </c>
@@ -10850,7 +10863,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>620</v>
       </c>
@@ -10876,7 +10889,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>623</v>
       </c>
@@ -10902,7 +10915,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>622</v>
       </c>
@@ -10928,7 +10941,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>621</v>
       </c>
@@ -10954,7 +10967,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>624</v>
       </c>
@@ -10980,7 +10993,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>625</v>
       </c>
@@ -11006,7 +11019,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>626</v>
       </c>
@@ -11032,7 +11045,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>627</v>
       </c>
@@ -11058,7 +11071,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>628</v>
       </c>
@@ -11084,7 +11097,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>629</v>
       </c>
@@ -11110,7 +11123,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>630</v>
       </c>
@@ -11136,7 +11149,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>631</v>
       </c>
@@ -11162,7 +11175,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>632</v>
       </c>
@@ -11188,7 +11201,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>633</v>
       </c>
@@ -11214,7 +11227,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>634</v>
       </c>
@@ -11240,7 +11253,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>635</v>
       </c>
@@ -11266,7 +11279,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>636</v>
       </c>
@@ -11292,7 +11305,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>637</v>
       </c>
@@ -11318,7 +11331,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>638</v>
       </c>
@@ -11344,7 +11357,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>639</v>
       </c>
@@ -11370,7 +11383,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>640</v>
       </c>
@@ -11396,7 +11409,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>641</v>
       </c>
@@ -11422,7 +11435,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>642</v>
       </c>
@@ -11448,7 +11461,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>643</v>
       </c>
@@ -11474,7 +11487,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>644</v>
       </c>
@@ -11500,7 +11513,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>645</v>
       </c>
@@ -11526,7 +11539,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>646</v>
       </c>
@@ -11552,7 +11565,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>647</v>
       </c>
@@ -11578,7 +11591,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>648</v>
       </c>
@@ -11604,7 +11617,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>649</v>
       </c>
@@ -11630,7 +11643,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>650</v>
       </c>
@@ -11656,7 +11669,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>651</v>
       </c>
@@ -11682,7 +11695,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>652</v>
       </c>
@@ -11708,7 +11721,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>654</v>
       </c>
@@ -11734,7 +11747,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>653</v>
       </c>
@@ -11760,7 +11773,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>655</v>
       </c>
@@ -11786,7 +11799,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>656</v>
       </c>
@@ -11812,7 +11825,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>867</v>
       </c>
@@ -11838,7 +11851,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>702</v>
       </c>
@@ -11864,7 +11877,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>703</v>
       </c>
@@ -11890,7 +11903,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>657</v>
       </c>
@@ -11916,7 +11929,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>658</v>
       </c>
@@ -11942,7 +11955,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>270</v>
       </c>
@@ -11968,7 +11981,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>271</v>
       </c>
@@ -11994,7 +12007,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>272</v>
       </c>
@@ -12020,7 +12033,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>81</v>
       </c>
@@ -12044,7 +12057,7 @@
       </c>
       <c r="K285" s="3"/>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>40</v>
       </c>
@@ -12070,7 +12083,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>72</v>
       </c>
@@ -12093,7 +12106,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>39</v>
       </c>
@@ -12119,7 +12132,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>69</v>
       </c>
@@ -12145,7 +12158,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>170</v>
       </c>
@@ -12168,7 +12181,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>178</v>
       </c>
@@ -12188,7 +12201,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>187</v>
       </c>
@@ -12208,7 +12221,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>71</v>
       </c>
@@ -12228,7 +12241,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>70</v>
       </c>
@@ -12248,7 +12261,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>76</v>
       </c>
@@ -12268,7 +12281,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>75</v>
       </c>
@@ -12288,7 +12301,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>74</v>
       </c>
@@ -12308,7 +12321,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>88</v>
       </c>
@@ -12328,7 +12341,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>89</v>
       </c>
@@ -12348,7 +12361,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>50</v>
       </c>
@@ -12368,7 +12381,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>188</v>
       </c>
@@ -12388,7 +12401,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>177</v>
       </c>
@@ -12408,7 +12421,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>26</v>
       </c>
@@ -12428,7 +12441,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>95</v>
       </c>
@@ -12448,7 +12461,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>94</v>
       </c>
@@ -12468,7 +12481,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>97</v>
       </c>
@@ -12488,7 +12501,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>96</v>
       </c>
@@ -12508,7 +12521,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>10</v>
       </c>
@@ -12528,7 +12541,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>84</v>
       </c>
@@ -12548,7 +12561,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>83</v>
       </c>
@@ -12568,7 +12581,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>38</v>
       </c>
@@ -12594,7 +12607,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>183</v>
       </c>
@@ -12620,7 +12633,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>263</v>
       </c>
@@ -12646,7 +12659,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>17</v>
       </c>
@@ -12672,7 +12685,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>260</v>
       </c>
@@ -12699,7 +12712,7 @@
       </c>
       <c r="K315" s="3"/>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>262</v>
       </c>
@@ -12725,7 +12738,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>261</v>
       </c>
@@ -12751,7 +12764,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>264</v>
       </c>
@@ -12777,7 +12790,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>115</v>
       </c>
@@ -12803,7 +12816,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>184</v>
       </c>
@@ -12826,7 +12839,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>18</v>
       </c>
@@ -12849,7 +12862,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>19</v>
       </c>
@@ -12872,7 +12885,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>133</v>
       </c>
@@ -12892,7 +12905,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>14</v>
       </c>
@@ -12912,7 +12925,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>15</v>
       </c>
@@ -12932,7 +12945,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>4</v>
       </c>
@@ -12952,7 +12965,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>20</v>
       </c>
@@ -12972,7 +12985,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>31</v>
       </c>
@@ -12992,7 +13005,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>27</v>
       </c>
@@ -13012,7 +13025,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>550</v>
       </c>
@@ -13038,7 +13051,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>165</v>
       </c>
@@ -13061,7 +13074,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>93</v>
       </c>
@@ -13084,7 +13097,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>91</v>
       </c>
@@ -13107,7 +13120,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>90</v>
       </c>
@@ -13128,6 +13141,28 @@
       </c>
       <c r="J334" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>941</v>
+      </c>
+      <c r="B335" t="s">
+        <v>106</v>
+      </c>
+      <c r="D335" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>943</v>
+      </c>
+      <c r="B336" t="s">
+        <v>106</v>
+      </c>
+      <c r="D336" t="s">
+        <v>944</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add final names in variable list file
</commit_message>
<xml_diff>
--- a/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
+++ b/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkim4\Documents\GitHub\ComStock\measures\comstock_sensitivity_reports\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D5FB5D-3D5E-47DD-8948-C310BBB7A524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB007D4-F293-42DB-BA5F-BF97C7D083BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -2865,16 +2865,16 @@
     <t>com_report_hvac_vrf_heating_design_cop_minus_22_f</t>
   </si>
   <si>
-    <t>Heat pump heating cycling ratio weighted by heating rate</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_heating_cycling_ratio</t>
-  </si>
-  <si>
-    <t>Heat pump cooling cycling ratio weighted by cooling rate</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_cycling_ratio</t>
+    <t>com_report_unitary_sys_cycling_ratio_cooling</t>
+  </si>
+  <si>
+    <t>com_report_unitary_sys_cycling_ratio_heating</t>
+  </si>
+  <si>
+    <t>Weighted average unitary system cycling ratio for heating</t>
+  </si>
+  <si>
+    <t>Weighted average unitary system cycling ratio for cooling</t>
   </si>
 </sst>
 </file>
@@ -4692,8 +4692,8 @@
   <dimension ref="A1:K336"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D335" sqref="D335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13145,7 +13145,7 @@
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="B335" t="s">
         <v>106</v>
@@ -13156,13 +13156,13 @@
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B336" t="s">
         <v>106</v>
       </c>
       <c r="D336" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding cycling output var in variable list excel file
</commit_message>
<xml_diff>
--- a/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
+++ b/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdahlhau\Documents\GitHub\NREL\comstock\measures\comstock_sensitivity_reports\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkim4\Documents\GitHub\ComStock\measures\comstock_sensitivity_reports\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512E82F8-75E4-4D3D-92A6-570946936AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B87A69C-A65F-4FA4-B756-51B6FF8AFACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="949">
   <si>
     <t>Input List</t>
   </si>
@@ -2875,6 +2875,18 @@
   </si>
   <si>
     <t>number of ThermalZone objects with multipliers</t>
+  </si>
+  <si>
+    <t>Weighted average unitary system cycling ratio for heating</t>
+  </si>
+  <si>
+    <t>com_report_unitary_sys_cycling_ratio_heating</t>
+  </si>
+  <si>
+    <t>Weighted average unitary system cycling ratio for cooling</t>
+  </si>
+  <si>
+    <t>com_report_unitary_sys_cycling_ratio_cooling</t>
   </si>
 </sst>
 </file>
@@ -3334,16 +3346,16 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3363,7 +3375,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3380,7 +3392,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3394,7 +3406,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3408,7 +3420,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -3422,7 +3434,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3436,7 +3448,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3450,7 +3462,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3464,7 +3476,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3478,7 +3490,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3492,7 +3504,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -3506,7 +3518,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3523,7 +3535,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -3537,7 +3549,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3551,7 +3563,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3565,7 +3577,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -3582,7 +3594,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3596,7 +3608,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3610,7 +3622,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3624,7 +3636,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3638,7 +3650,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3655,7 +3667,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -3669,7 +3681,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>112</v>
       </c>
@@ -3686,7 +3698,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3703,7 +3715,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -3717,7 +3729,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3734,7 +3746,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3751,7 +3763,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -3765,7 +3777,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -3779,7 +3791,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3796,7 +3808,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3810,7 +3822,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3827,7 +3839,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -3841,7 +3853,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3858,7 +3870,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -3872,7 +3884,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3886,7 +3898,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -3903,7 +3915,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -3917,7 +3929,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3931,7 +3943,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3945,7 +3957,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -3959,7 +3971,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -3973,7 +3985,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -3987,7 +3999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -4001,7 +4013,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -4018,7 +4030,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>108</v>
       </c>
@@ -4032,7 +4044,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4049,7 +4061,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -4063,7 +4075,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -4077,7 +4089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -4091,7 +4103,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -4108,7 +4120,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4122,7 +4134,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -4136,7 +4148,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -4150,7 +4162,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -4164,7 +4176,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4181,7 +4193,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -4195,7 +4207,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -4209,7 +4221,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -4223,7 +4235,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -4237,7 +4249,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -4251,7 +4263,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -4265,7 +4277,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -4279,7 +4291,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -4293,7 +4305,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -4307,7 +4319,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -4321,7 +4333,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -4338,7 +4350,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -4352,7 +4364,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4366,7 +4378,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -4383,7 +4395,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -4397,7 +4409,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -4411,7 +4423,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -4425,7 +4437,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -4442,7 +4454,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -4459,7 +4471,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -4473,7 +4485,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -4487,7 +4499,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -4501,7 +4513,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -4515,7 +4527,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -4529,7 +4541,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -4543,7 +4555,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -4557,7 +4569,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4571,7 +4583,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -4588,7 +4600,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -4602,7 +4614,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -4616,7 +4628,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -4633,7 +4645,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -4647,7 +4659,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -4664,7 +4676,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>133</v>
       </c>
@@ -4689,28 +4701,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE568D5-2279-4922-8B77-550F2E5B90B6}">
-  <dimension ref="A1:K336"/>
+  <dimension ref="A1:K338"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A319" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A337" sqref="A337:XFD338"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="102" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>176</v>
       </c>
@@ -4745,7 +4757,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>525</v>
       </c>
@@ -4771,7 +4783,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>526</v>
       </c>
@@ -4797,7 +4809,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>523</v>
       </c>
@@ -4823,7 +4835,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>524</v>
       </c>
@@ -4849,7 +4861,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>533</v>
       </c>
@@ -4875,7 +4887,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>453</v>
       </c>
@@ -4901,7 +4913,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>455</v>
       </c>
@@ -4927,7 +4939,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>454</v>
       </c>
@@ -4953,7 +4965,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>534</v>
       </c>
@@ -4979,7 +4991,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>452</v>
       </c>
@@ -5005,7 +5017,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -5028,7 +5040,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -5057,7 +5069,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>254</v>
       </c>
@@ -5077,7 +5089,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>255</v>
       </c>
@@ -5097,7 +5109,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>942</v>
       </c>
@@ -5120,7 +5132,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>936</v>
       </c>
@@ -5146,7 +5158,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>941</v>
       </c>
@@ -5169,7 +5181,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>938</v>
       </c>
@@ -5195,7 +5207,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>939</v>
       </c>
@@ -5221,7 +5233,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>937</v>
       </c>
@@ -5247,7 +5259,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -5273,7 +5285,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -5299,7 +5311,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -5325,7 +5337,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>475</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -5380,7 +5392,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>472</v>
       </c>
@@ -5406,7 +5418,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>479</v>
       </c>
@@ -5432,7 +5444,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -5458,7 +5470,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -5484,7 +5496,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -5510,7 +5522,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -5536,7 +5548,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -5559,7 +5571,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -5582,7 +5594,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -5605,7 +5617,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -5628,7 +5640,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -5654,7 +5666,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -5674,7 +5686,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -5694,7 +5706,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -5714,7 +5726,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -5734,7 +5746,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -5754,7 +5766,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -5774,7 +5786,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -5794,7 +5806,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -5814,7 +5826,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -5834,7 +5846,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -5854,7 +5866,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>266</v>
       </c>
@@ -5880,7 +5892,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>268</v>
       </c>
@@ -5906,7 +5918,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>267</v>
       </c>
@@ -5932,7 +5944,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>230</v>
       </c>
@@ -5958,7 +5970,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>231</v>
       </c>
@@ -5984,7 +5996,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>233</v>
       </c>
@@ -6010,7 +6022,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>232</v>
       </c>
@@ -6036,7 +6048,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>199</v>
       </c>
@@ -6062,7 +6074,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>205</v>
       </c>
@@ -6089,7 +6101,7 @@
       </c>
       <c r="K56" s="3"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>206</v>
       </c>
@@ -6116,7 +6128,7 @@
       </c>
       <c r="K57" s="3"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>265</v>
       </c>
@@ -6142,7 +6154,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>777</v>
       </c>
@@ -6168,7 +6180,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>781</v>
       </c>
@@ -6194,7 +6206,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>776</v>
       </c>
@@ -6220,7 +6232,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>775</v>
       </c>
@@ -6246,7 +6258,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>388</v>
       </c>
@@ -6272,7 +6284,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>393</v>
       </c>
@@ -6298,7 +6310,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>394</v>
       </c>
@@ -6324,7 +6336,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>389</v>
       </c>
@@ -6350,7 +6362,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>390</v>
       </c>
@@ -6376,7 +6388,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -6402,7 +6414,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>392</v>
       </c>
@@ -6428,7 +6440,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>729</v>
       </c>
@@ -6454,7 +6466,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>730</v>
       </c>
@@ -6480,7 +6492,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>733</v>
       </c>
@@ -6506,7 +6518,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>731</v>
       </c>
@@ -6532,7 +6544,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>732</v>
       </c>
@@ -6558,7 +6570,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>735</v>
       </c>
@@ -6584,7 +6596,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>734</v>
       </c>
@@ -6610,7 +6622,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>737</v>
       </c>
@@ -6636,7 +6648,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>738</v>
       </c>
@@ -6662,7 +6674,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>736</v>
       </c>
@@ -6688,7 +6700,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>741</v>
       </c>
@@ -6714,7 +6726,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>739</v>
       </c>
@@ -6740,7 +6752,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>740</v>
       </c>
@@ -6766,7 +6778,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>742</v>
       </c>
@@ -6792,7 +6804,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>743</v>
       </c>
@@ -6818,7 +6830,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>744</v>
       </c>
@@ -6844,7 +6856,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>916</v>
       </c>
@@ -6870,7 +6882,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>917</v>
       </c>
@@ -6896,7 +6908,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>919</v>
       </c>
@@ -6922,7 +6934,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>918</v>
       </c>
@@ -6948,7 +6960,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>920</v>
       </c>
@@ -6974,7 +6986,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>921</v>
       </c>
@@ -7000,7 +7012,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>746</v>
       </c>
@@ -7026,7 +7038,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>745</v>
       </c>
@@ -7052,7 +7064,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>752</v>
       </c>
@@ -7078,7 +7090,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>747</v>
       </c>
@@ -7104,7 +7116,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>795</v>
       </c>
@@ -7130,7 +7142,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>796</v>
       </c>
@@ -7156,7 +7168,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>797</v>
       </c>
@@ -7182,7 +7194,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>798</v>
       </c>
@@ -7208,7 +7220,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>748</v>
       </c>
@@ -7234,7 +7246,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>791</v>
       </c>
@@ -7260,7 +7272,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>792</v>
       </c>
@@ -7286,7 +7298,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>793</v>
       </c>
@@ -7312,7 +7324,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>794</v>
       </c>
@@ -7338,7 +7350,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>808</v>
       </c>
@@ -7364,7 +7376,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>274</v>
       </c>
@@ -7390,7 +7402,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>576</v>
       </c>
@@ -7416,7 +7428,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>552</v>
       </c>
@@ -7442,7 +7454,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>575</v>
       </c>
@@ -7468,7 +7480,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>574</v>
       </c>
@@ -7494,7 +7506,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>588</v>
       </c>
@@ -7520,7 +7532,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>586</v>
       </c>
@@ -7546,7 +7558,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>585</v>
       </c>
@@ -7572,7 +7584,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>587</v>
       </c>
@@ -7598,7 +7610,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>556</v>
       </c>
@@ -7624,7 +7636,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>77</v>
       </c>
@@ -7650,7 +7662,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>340</v>
       </c>
@@ -7676,7 +7688,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>483</v>
       </c>
@@ -7702,7 +7714,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>281</v>
       </c>
@@ -7728,7 +7740,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>283</v>
       </c>
@@ -7754,7 +7766,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>282</v>
       </c>
@@ -7780,7 +7792,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>276</v>
       </c>
@@ -7806,7 +7818,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -7832,7 +7844,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>279</v>
       </c>
@@ -7858,7 +7870,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>280</v>
       </c>
@@ -7884,7 +7896,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>277</v>
       </c>
@@ -7910,7 +7922,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>309</v>
       </c>
@@ -7936,7 +7948,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>313</v>
       </c>
@@ -7962,7 +7974,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>312</v>
       </c>
@@ -7988,7 +8000,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>310</v>
       </c>
@@ -8014,7 +8026,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>311</v>
       </c>
@@ -8040,7 +8052,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>314</v>
       </c>
@@ -8066,7 +8078,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>288</v>
       </c>
@@ -8095,7 +8107,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>290</v>
       </c>
@@ -8124,7 +8136,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>291</v>
       </c>
@@ -8153,7 +8165,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>289</v>
       </c>
@@ -8182,7 +8194,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>402</v>
       </c>
@@ -8211,7 +8223,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>292</v>
       </c>
@@ -8237,7 +8249,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>295</v>
       </c>
@@ -8263,7 +8275,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>296</v>
       </c>
@@ -8289,7 +8301,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>293</v>
       </c>
@@ -8315,7 +8327,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>294</v>
       </c>
@@ -8341,7 +8353,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>592</v>
       </c>
@@ -8367,7 +8379,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>591</v>
       </c>
@@ -8393,7 +8405,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>590</v>
       </c>
@@ -8419,7 +8431,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>589</v>
       </c>
@@ -8445,7 +8457,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>247</v>
       </c>
@@ -8472,7 +8484,7 @@
       </c>
       <c r="K147" s="3"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
         <v>106</v>
       </c>
@@ -8496,7 +8508,7 @@
       </c>
       <c r="K148" s="3"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>880</v>
       </c>
@@ -8523,7 +8535,7 @@
       </c>
       <c r="K149" s="3"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>883</v>
       </c>
@@ -8550,7 +8562,7 @@
       </c>
       <c r="K150" s="3"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>106</v>
       </c>
@@ -8574,7 +8586,7 @@
       </c>
       <c r="K151" s="3"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
         <v>106</v>
       </c>
@@ -8598,7 +8610,7 @@
       </c>
       <c r="K152" s="3"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>106</v>
       </c>
@@ -8622,7 +8634,7 @@
       </c>
       <c r="K153" s="3"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>881</v>
       </c>
@@ -8649,7 +8661,7 @@
       </c>
       <c r="K154" s="3"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>882</v>
       </c>
@@ -8676,7 +8688,7 @@
       </c>
       <c r="K155" s="3"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>106</v>
       </c>
@@ -8700,7 +8712,7 @@
       </c>
       <c r="K156" s="3"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>106</v>
       </c>
@@ -8724,7 +8736,7 @@
       </c>
       <c r="K157" s="3"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>273</v>
       </c>
@@ -8750,7 +8762,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>316</v>
       </c>
@@ -8776,7 +8788,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>246</v>
       </c>
@@ -8802,7 +8814,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>441</v>
       </c>
@@ -8828,7 +8840,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>443</v>
       </c>
@@ -8854,7 +8866,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>439</v>
       </c>
@@ -8880,7 +8892,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>445</v>
       </c>
@@ -8906,7 +8918,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>442</v>
       </c>
@@ -8932,7 +8944,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>444</v>
       </c>
@@ -8958,7 +8970,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>440</v>
       </c>
@@ -8984,7 +8996,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>446</v>
       </c>
@@ -9010,7 +9022,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>437</v>
       </c>
@@ -9036,7 +9048,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>438</v>
       </c>
@@ -9062,7 +9074,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>505</v>
       </c>
@@ -9088,7 +9100,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>510</v>
       </c>
@@ -9114,7 +9126,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>275</v>
       </c>
@@ -9140,7 +9152,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>345</v>
       </c>
@@ -9166,7 +9178,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>275</v>
       </c>
@@ -9192,7 +9204,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>484</v>
       </c>
@@ -9218,7 +9230,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>353</v>
       </c>
@@ -9244,7 +9256,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>354</v>
       </c>
@@ -9270,7 +9282,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>317</v>
       </c>
@@ -9296,7 +9308,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>456</v>
       </c>
@@ -9322,7 +9334,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>362</v>
       </c>
@@ -9348,7 +9360,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>487</v>
       </c>
@@ -9374,7 +9386,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>404</v>
       </c>
@@ -9400,7 +9412,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>363</v>
       </c>
@@ -9426,7 +9438,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>405</v>
       </c>
@@ -9452,7 +9464,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>364</v>
       </c>
@@ -9478,7 +9490,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>403</v>
       </c>
@@ -9504,7 +9516,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>400</v>
       </c>
@@ -9530,7 +9542,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>401</v>
       </c>
@@ -9556,7 +9568,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>512</v>
       </c>
@@ -9582,7 +9594,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>511</v>
       </c>
@@ -9608,7 +9620,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>450</v>
       </c>
@@ -9634,7 +9646,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>451</v>
       </c>
@@ -9660,7 +9672,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>369</v>
       </c>
@@ -9686,7 +9698,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>370</v>
       </c>
@@ -9712,7 +9724,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>368</v>
       </c>
@@ -9738,7 +9750,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>499</v>
       </c>
@@ -9764,7 +9776,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>583</v>
       </c>
@@ -9790,7 +9802,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>584</v>
       </c>
@@ -9816,7 +9828,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>501</v>
       </c>
@@ -9842,7 +9854,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>502</v>
       </c>
@@ -9868,7 +9880,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>500</v>
       </c>
@@ -9894,7 +9906,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>906</v>
       </c>
@@ -9920,7 +9932,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>907</v>
       </c>
@@ -9946,7 +9958,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>285</v>
       </c>
@@ -9972,7 +9984,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>830</v>
       </c>
@@ -9998,7 +10010,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>832</v>
       </c>
@@ -10024,7 +10036,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>834</v>
       </c>
@@ -10050,7 +10062,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>836</v>
       </c>
@@ -10076,7 +10088,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>838</v>
       </c>
@@ -10102,7 +10114,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>840</v>
       </c>
@@ -10128,7 +10140,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>843</v>
       </c>
@@ -10154,7 +10166,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>848</v>
       </c>
@@ -10180,7 +10192,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>815</v>
       </c>
@@ -10206,7 +10218,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>816</v>
       </c>
@@ -10232,7 +10244,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>820</v>
       </c>
@@ -10258,7 +10270,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>817</v>
       </c>
@@ -10284,7 +10296,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>818</v>
       </c>
@@ -10310,7 +10322,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>819</v>
       </c>
@@ -10336,7 +10348,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>826</v>
       </c>
@@ -10362,7 +10374,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>827</v>
       </c>
@@ -10388,7 +10400,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>829</v>
       </c>
@@ -10414,7 +10426,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>828</v>
       </c>
@@ -10440,7 +10452,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>849</v>
       </c>
@@ -10466,7 +10478,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>901</v>
       </c>
@@ -10492,7 +10504,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>902</v>
       </c>
@@ -10518,7 +10530,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>903</v>
       </c>
@@ -10544,7 +10556,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>857</v>
       </c>
@@ -10570,7 +10582,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>858</v>
       </c>
@@ -10596,7 +10608,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>859</v>
       </c>
@@ -10622,7 +10634,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>860</v>
       </c>
@@ -10648,7 +10660,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>861</v>
       </c>
@@ -10674,7 +10686,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>341</v>
       </c>
@@ -10700,7 +10712,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>561</v>
       </c>
@@ -10726,7 +10738,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>562</v>
       </c>
@@ -10752,7 +10764,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>560</v>
       </c>
@@ -10778,7 +10790,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>468</v>
       </c>
@@ -10804,7 +10816,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>469</v>
       </c>
@@ -10830,7 +10842,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>470</v>
       </c>
@@ -10856,7 +10868,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>471</v>
       </c>
@@ -10882,7 +10894,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>619</v>
       </c>
@@ -10908,7 +10920,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>620</v>
       </c>
@@ -10934,7 +10946,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>623</v>
       </c>
@@ -10960,7 +10972,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>622</v>
       </c>
@@ -10986,7 +10998,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>621</v>
       </c>
@@ -11012,7 +11024,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>624</v>
       </c>
@@ -11038,7 +11050,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>625</v>
       </c>
@@ -11064,7 +11076,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>626</v>
       </c>
@@ -11090,7 +11102,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>627</v>
       </c>
@@ -11116,7 +11128,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>628</v>
       </c>
@@ -11142,7 +11154,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>629</v>
       </c>
@@ -11168,7 +11180,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>630</v>
       </c>
@@ -11194,7 +11206,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>631</v>
       </c>
@@ -11220,7 +11232,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>632</v>
       </c>
@@ -11246,7 +11258,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>633</v>
       </c>
@@ -11272,7 +11284,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>634</v>
       </c>
@@ -11298,7 +11310,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>635</v>
       </c>
@@ -11324,7 +11336,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>636</v>
       </c>
@@ -11350,7 +11362,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>637</v>
       </c>
@@ -11376,7 +11388,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>638</v>
       </c>
@@ -11402,7 +11414,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>639</v>
       </c>
@@ -11428,7 +11440,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>640</v>
       </c>
@@ -11454,7 +11466,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>641</v>
       </c>
@@ -11480,7 +11492,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>642</v>
       </c>
@@ -11506,7 +11518,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>643</v>
       </c>
@@ -11532,7 +11544,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>644</v>
       </c>
@@ -11558,7 +11570,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>645</v>
       </c>
@@ -11584,7 +11596,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>646</v>
       </c>
@@ -11610,7 +11622,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>647</v>
       </c>
@@ -11636,7 +11648,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>648</v>
       </c>
@@ -11662,7 +11674,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>649</v>
       </c>
@@ -11688,7 +11700,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>650</v>
       </c>
@@ -11714,7 +11726,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>651</v>
       </c>
@@ -11740,7 +11752,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>652</v>
       </c>
@@ -11766,7 +11778,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>654</v>
       </c>
@@ -11792,7 +11804,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>653</v>
       </c>
@@ -11818,7 +11830,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>655</v>
       </c>
@@ -11844,7 +11856,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>656</v>
       </c>
@@ -11870,7 +11882,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>867</v>
       </c>
@@ -11896,7 +11908,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>702</v>
       </c>
@@ -11922,7 +11934,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>703</v>
       </c>
@@ -11948,7 +11960,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>657</v>
       </c>
@@ -11974,7 +11986,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>658</v>
       </c>
@@ -12000,7 +12012,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>270</v>
       </c>
@@ -12026,7 +12038,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>271</v>
       </c>
@@ -12052,7 +12064,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>272</v>
       </c>
@@ -12078,7 +12090,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>81</v>
       </c>
@@ -12102,7 +12114,7 @@
       </c>
       <c r="K287" s="3"/>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>40</v>
       </c>
@@ -12128,7 +12140,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>72</v>
       </c>
@@ -12151,7 +12163,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>39</v>
       </c>
@@ -12177,7 +12189,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>69</v>
       </c>
@@ -12203,7 +12215,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>170</v>
       </c>
@@ -12226,7 +12238,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>178</v>
       </c>
@@ -12246,7 +12258,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>187</v>
       </c>
@@ -12266,7 +12278,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>71</v>
       </c>
@@ -12286,7 +12298,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>70</v>
       </c>
@@ -12306,7 +12318,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>76</v>
       </c>
@@ -12326,7 +12338,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>75</v>
       </c>
@@ -12346,7 +12358,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>74</v>
       </c>
@@ -12366,7 +12378,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>88</v>
       </c>
@@ -12386,7 +12398,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>89</v>
       </c>
@@ -12406,7 +12418,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>50</v>
       </c>
@@ -12426,7 +12438,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>188</v>
       </c>
@@ -12446,7 +12458,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>177</v>
       </c>
@@ -12466,7 +12478,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>26</v>
       </c>
@@ -12486,7 +12498,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>95</v>
       </c>
@@ -12506,7 +12518,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>94</v>
       </c>
@@ -12526,7 +12538,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>97</v>
       </c>
@@ -12546,7 +12558,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>96</v>
       </c>
@@ -12566,7 +12578,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>10</v>
       </c>
@@ -12586,7 +12598,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>84</v>
       </c>
@@ -12606,7 +12618,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>83</v>
       </c>
@@ -12626,7 +12638,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>38</v>
       </c>
@@ -12652,7 +12664,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>183</v>
       </c>
@@ -12678,7 +12690,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>263</v>
       </c>
@@ -12704,7 +12716,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>17</v>
       </c>
@@ -12730,7 +12742,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>260</v>
       </c>
@@ -12757,7 +12769,7 @@
       </c>
       <c r="K317" s="3"/>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>262</v>
       </c>
@@ -12783,7 +12795,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>261</v>
       </c>
@@ -12809,7 +12821,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>264</v>
       </c>
@@ -12835,7 +12847,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>115</v>
       </c>
@@ -12861,7 +12873,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>184</v>
       </c>
@@ -12884,7 +12896,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>18</v>
       </c>
@@ -12907,7 +12919,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>19</v>
       </c>
@@ -12930,7 +12942,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>133</v>
       </c>
@@ -12950,7 +12962,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>14</v>
       </c>
@@ -12970,7 +12982,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>15</v>
       </c>
@@ -12990,7 +13002,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>4</v>
       </c>
@@ -13010,7 +13022,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>20</v>
       </c>
@@ -13030,7 +13042,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>31</v>
       </c>
@@ -13050,7 +13062,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>27</v>
       </c>
@@ -13070,7 +13082,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>550</v>
       </c>
@@ -13096,7 +13108,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>165</v>
       </c>
@@ -13119,7 +13131,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>93</v>
       </c>
@@ -13142,7 +13154,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>91</v>
       </c>
@@ -13165,7 +13177,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>90</v>
       </c>
@@ -13186,6 +13198,28 @@
       </c>
       <c r="J336" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>945</v>
+      </c>
+      <c r="B337" t="s">
+        <v>106</v>
+      </c>
+      <c r="D337" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>947</v>
+      </c>
+      <c r="B338" t="s">
+        <v>106</v>
+      </c>
+      <c r="D338" t="s">
+        <v>948</v>
       </c>
     </row>
   </sheetData>
@@ -13194,7 +13228,7 @@
       <sortCondition ref="B1:B336"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="J86:J91 J105 J148 J213 E2:E336 J16:J21 H2:I336">
+  <conditionalFormatting sqref="E2:E336 H2:I336 J16:J21 J86:J91 J105 J148 J213">
     <cfRule type="containsText" dxfId="9" priority="38" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
water to water heat pump outputs fix
modified generic heat pump output variables to include water-to-water in the name. the output variables now follow the water-to-air naming convention - "ww_hp". change implemented in 4 files:
- measure.rb
- measure.xml
- Variable List.xlsx
- comstock_column_definitions.csv
</commit_message>
<xml_diff>
--- a/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
+++ b/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdahlhau\Documents\GitHub\NREL\comstock\measures\comstock_sensitivity_reports\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alebar\Documents\GitHub\ComStock\measures\comstock_sensitivity_reports\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C3DA4A-23E1-48DA-A20C-E70AF45504F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BA88F2-09AF-4F13-94EC-4AF1D3E934C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="1620" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -2469,129 +2469,15 @@
     <t>HVAC VRF outdoor temperature type use for eir performance curves</t>
   </si>
   <si>
-    <t>com_report_hvac_heat_pump_heating_total_load_j</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_heating_total_electric_j</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_heating_capacity_kbtuh</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_heating_average_cop</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_heating_capacity_weighted_design_cop</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_heating_load_weighted_design_cop</t>
-  </si>
-  <si>
-    <t>Heat pump heating load weighted average cop</t>
-  </si>
-  <si>
-    <t>Heat pump heating capacity</t>
-  </si>
-  <si>
-    <t>Heat pump heating load weighted design cop</t>
-  </si>
-  <si>
-    <t>Heat pump heating electric use</t>
-  </si>
-  <si>
-    <t>Heat pump heating heating load served</t>
-  </si>
-  <si>
-    <t>Heat pump heating capacity weighted design cop</t>
-  </si>
-  <si>
-    <t>com_report_hvac_count_heat_pumps_heating</t>
-  </si>
-  <si>
-    <t>com_report_hvac_count_heat_pumps_heating_0_to_300_kbtuh</t>
-  </si>
-  <si>
-    <t>com_report_hvac_count_heat_pumps_heating_300_to_2500_kbtuh</t>
-  </si>
-  <si>
-    <t>com_report_hvac_count_heat_pumps_heating_2500_plus_kbtuh</t>
-  </si>
-  <si>
     <t>number of heat pumps for heating</t>
   </si>
   <si>
-    <t>Number of heat pumps for heating</t>
-  </si>
-  <si>
-    <t>Number of heat pumps for heating between 0 and 300 kbtuh</t>
-  </si>
-  <si>
-    <t>Number of heat pumps for heating larger than 2500 kbtuh</t>
-  </si>
-  <si>
-    <t>Number of heat pumps for heating between 300 and 2500 kbtuh</t>
-  </si>
-  <si>
-    <t>Heat pump cooling load weighted average cop</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_average_cop</t>
-  </si>
-  <si>
-    <t>Heat pump cooling capacity</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_capacity_kbtuh</t>
-  </si>
-  <si>
-    <t>Heat pump cooling capacity weighted design cop</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_capacity_weighted_design_cop</t>
-  </si>
-  <si>
-    <t>Heat pump cooling load weighted design cop</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_load_weighted_design_cop</t>
-  </si>
-  <si>
-    <t>Heat pump cooling electric use</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_total_electric_j</t>
-  </si>
-  <si>
-    <t>Heat pump cooling cooling load served</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_total_load_j</t>
-  </si>
-  <si>
     <t>total heat pump cooling load served</t>
   </si>
   <si>
-    <t>Number of heat pumps for cooling</t>
-  </si>
-  <si>
-    <t>com_report_hvac_count_heat_pumps_cooling</t>
-  </si>
-  <si>
     <t>number of heat pumps for cooling</t>
   </si>
   <si>
-    <t>com_report_hvac_heat_pump_heating_load_weighted_source_inlet_temperature_c</t>
-  </si>
-  <si>
-    <t>com_report_hvac_heat_pump_cooling_load_weighted_source_inlet_temperature_c</t>
-  </si>
-  <si>
-    <t>Heat pump cooling source inlet temperature</t>
-  </si>
-  <si>
-    <t>Heat pump heating source inlet temperature</t>
-  </si>
-  <si>
     <t>heat pump cooling load weighted annual average source inlet temperature</t>
   </si>
   <si>
@@ -2896,6 +2782,120 @@
   </si>
   <si>
     <t>total water use from cooling towers includeing evaporation, drift, and blowdown</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_average_cop</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_capacity_kbtuh</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_capacity_weighted_design_cop</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_load_weighted_design_cop</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_total_electric_j</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_total_load_j</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_cooling_load_weighted_source_inlet_temperature_c</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_average_cop</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_capacity_kbtuh</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_capacity_weighted_design_cop</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_load_weighted_design_cop</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_total_electric_j</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_total_load_j</t>
+  </si>
+  <si>
+    <t>com_report_hvac_water_water_heat_pump_heating_load_weighted_source_inlet_temperature_c</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling load weighted average cop</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling capacity</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling capacity weighted design cop</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling load weighted design cop</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling electric use</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling cooling load served</t>
+  </si>
+  <si>
+    <t>Water to water heat pump cooling source inlet temperature</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating load weighted average cop</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating capacity</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating capacity weighted design cop</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating load weighted design cop</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating electric use</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating heating load served</t>
+  </si>
+  <si>
+    <t>Water to water heat pump heating source inlet temperature</t>
+  </si>
+  <si>
+    <t>com_report_hvac_count_water_water_heat_pumps_heating</t>
+  </si>
+  <si>
+    <t>com_report_hvac_count_water_water_heat_pumps_heating_0_to_300_kbtuh</t>
+  </si>
+  <si>
+    <t>com_report_hvac_count_water_water_heat_pumps_heating_300_to_2500_kbtuh</t>
+  </si>
+  <si>
+    <t>com_report_hvac_count_water_water_heat_pumps_heating_2500_plus_kbtuh</t>
+  </si>
+  <si>
+    <t>com_report_hvac_count_water_water_heat_pumps_cooling</t>
+  </si>
+  <si>
+    <t>Number of water to water heat pumps for cooling</t>
+  </si>
+  <si>
+    <t>Number of water to water heat pumps for heating</t>
+  </si>
+  <si>
+    <t>Number of water to water heat pumps for heating between 0 and 300 kbtuh</t>
+  </si>
+  <si>
+    <t>Number of water to water heat pumps for heating between 300 and 2500 kbtuh</t>
+  </si>
+  <si>
+    <t>Number of water to water heat pumps for heating larger than 2500 kbtuh</t>
   </si>
 </sst>
 </file>
@@ -3355,16 +3355,16 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>112</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>108</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>133</v>
       </c>
@@ -4712,26 +4712,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE568D5-2279-4922-8B77-550F2E5B90B6}">
   <dimension ref="A1:K339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D214" sqref="D214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="102" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>176</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>525</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>526</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>523</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>524</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>533</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>453</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>455</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>454</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>534</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>452</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>254</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>255</v>
       </c>
@@ -5118,9 +5118,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>942</v>
+        <v>904</v>
       </c>
       <c r="B16" t="s">
         <v>253</v>
@@ -5138,18 +5138,18 @@
         <v>119</v>
       </c>
       <c r="J16" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>936</v>
+        <v>898</v>
       </c>
       <c r="B17" t="s">
         <v>253</v>
       </c>
       <c r="D17" t="s">
-        <v>932</v>
+        <v>894</v>
       </c>
       <c r="E17" t="s">
         <v>153</v>
@@ -5164,12 +5164,12 @@
         <v>119</v>
       </c>
       <c r="J17" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>941</v>
+        <v>903</v>
       </c>
       <c r="B18" t="s">
         <v>253</v>
@@ -5187,18 +5187,18 @@
         <v>119</v>
       </c>
       <c r="J18" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="B19" t="s">
         <v>253</v>
       </c>
       <c r="D19" t="s">
-        <v>933</v>
+        <v>895</v>
       </c>
       <c r="E19" t="s">
         <v>153</v>
@@ -5213,18 +5213,18 @@
         <v>119</v>
       </c>
       <c r="J19" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>939</v>
+        <v>901</v>
       </c>
       <c r="B20" t="s">
         <v>253</v>
       </c>
       <c r="D20" t="s">
-        <v>934</v>
+        <v>896</v>
       </c>
       <c r="E20" t="s">
         <v>153</v>
@@ -5239,18 +5239,18 @@
         <v>119</v>
       </c>
       <c r="J20" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>937</v>
+        <v>899</v>
       </c>
       <c r="B21" t="s">
         <v>253</v>
       </c>
       <c r="D21" t="s">
-        <v>935</v>
+        <v>897</v>
       </c>
       <c r="E21" t="s">
         <v>153</v>
@@ -5265,10 +5265,10 @@
         <v>119</v>
       </c>
       <c r="J21" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>475</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>472</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>479</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>266</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>268</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>267</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>230</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>231</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>233</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>232</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>199</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>205</v>
       </c>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="K56" s="3"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>206</v>
       </c>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="K57" s="3"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>265</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>777</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>781</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>776</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>775</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>388</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>393</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>394</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>389</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>390</v>
       </c>
@@ -6397,7 +6397,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>392</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>729</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>730</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>733</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>731</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>732</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>735</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>734</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>737</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>738</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>736</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>741</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>739</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>740</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>742</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>743</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>744</v>
       </c>
@@ -6865,15 +6865,15 @@
         <v>757</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>916</v>
+        <v>878</v>
       </c>
       <c r="B86" t="s">
         <v>106</v>
       </c>
       <c r="D86" t="s">
-        <v>910</v>
+        <v>872</v>
       </c>
       <c r="E86" t="s">
         <v>153</v>
@@ -6888,18 +6888,18 @@
         <v>119</v>
       </c>
       <c r="J86" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>917</v>
+        <v>879</v>
       </c>
       <c r="B87" t="s">
         <v>106</v>
       </c>
       <c r="D87" t="s">
-        <v>911</v>
+        <v>873</v>
       </c>
       <c r="E87" t="s">
         <v>153</v>
@@ -6914,18 +6914,18 @@
         <v>119</v>
       </c>
       <c r="J87" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>919</v>
+        <v>881</v>
       </c>
       <c r="B88" t="s">
         <v>106</v>
       </c>
       <c r="D88" t="s">
-        <v>912</v>
+        <v>874</v>
       </c>
       <c r="E88" t="s">
         <v>153</v>
@@ -6940,18 +6940,18 @@
         <v>119</v>
       </c>
       <c r="J88" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>918</v>
+        <v>880</v>
       </c>
       <c r="B89" t="s">
         <v>106</v>
       </c>
       <c r="D89" t="s">
-        <v>913</v>
+        <v>875</v>
       </c>
       <c r="E89" t="s">
         <v>153</v>
@@ -6966,18 +6966,18 @@
         <v>119</v>
       </c>
       <c r="J89" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>920</v>
+        <v>882</v>
       </c>
       <c r="B90" t="s">
         <v>106</v>
       </c>
       <c r="D90" t="s">
-        <v>914</v>
+        <v>876</v>
       </c>
       <c r="E90" t="s">
         <v>153</v>
@@ -6992,18 +6992,18 @@
         <v>119</v>
       </c>
       <c r="J90" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>921</v>
+        <v>883</v>
       </c>
       <c r="B91" t="s">
         <v>106</v>
       </c>
       <c r="D91" t="s">
-        <v>915</v>
+        <v>877</v>
       </c>
       <c r="E91" t="s">
         <v>153</v>
@@ -7018,10 +7018,10 @@
         <v>119</v>
       </c>
       <c r="J91" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>746</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>745</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>752</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>747</v>
       </c>
@@ -7125,7 +7125,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>795</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>796</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>797</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>798</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>748</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>791</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>106</v>
       </c>
       <c r="D101" t="s">
-        <v>940</v>
+        <v>902</v>
       </c>
       <c r="E101" t="s">
         <v>153</v>
@@ -7281,7 +7281,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>792</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>793</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>794</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>808</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>274</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>576</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>552</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>575</v>
       </c>
@@ -7489,7 +7489,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>574</v>
       </c>
@@ -7515,7 +7515,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>588</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>586</v>
       </c>
@@ -7567,7 +7567,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>585</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>587</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>556</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>77</v>
       </c>
@@ -7671,15 +7671,15 @@
         <v>300</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>949</v>
+        <v>911</v>
       </c>
       <c r="B117" t="s">
         <v>106</v>
       </c>
       <c r="D117" t="s">
-        <v>950</v>
+        <v>912</v>
       </c>
       <c r="E117" t="s">
         <v>119</v>
@@ -7694,10 +7694,10 @@
         <v>119</v>
       </c>
       <c r="J117" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>340</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>483</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>281</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>283</v>
       </c>
@@ -7801,7 +7801,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>282</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>276</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>278</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>279</v>
       </c>
@@ -7905,7 +7905,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>280</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>277</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>309</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>313</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>312</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>310</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>311</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>314</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>288</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>290</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>291</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>289</v>
       </c>
@@ -8229,7 +8229,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>402</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>292</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>295</v>
       </c>
@@ -8310,7 +8310,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>296</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>293</v>
       </c>
@@ -8362,7 +8362,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>294</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>592</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>591</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>590</v>
       </c>
@@ -8466,7 +8466,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>589</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>247</v>
       </c>
@@ -8519,12 +8519,12 @@
       </c>
       <c r="K148" s="3"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
         <v>106</v>
       </c>
       <c r="D149" t="s">
-        <v>870</v>
+        <v>832</v>
       </c>
       <c r="E149" t="s">
         <v>119</v>
@@ -8539,19 +8539,19 @@
         <v>119</v>
       </c>
       <c r="J149" t="s">
-        <v>889</v>
+        <v>851</v>
       </c>
       <c r="K149" s="3"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>880</v>
+        <v>842</v>
       </c>
       <c r="B150" t="s">
         <v>106</v>
       </c>
       <c r="D150" t="s">
-        <v>871</v>
+        <v>833</v>
       </c>
       <c r="E150" t="s">
         <v>119</v>
@@ -8566,19 +8566,19 @@
         <v>119</v>
       </c>
       <c r="J150" t="s">
-        <v>884</v>
+        <v>846</v>
       </c>
       <c r="K150" s="3"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>883</v>
+        <v>845</v>
       </c>
       <c r="B151" t="s">
         <v>106</v>
       </c>
       <c r="D151" t="s">
-        <v>872</v>
+        <v>834</v>
       </c>
       <c r="E151" t="s">
         <v>119</v>
@@ -8593,16 +8593,16 @@
         <v>119</v>
       </c>
       <c r="J151" t="s">
-        <v>887</v>
+        <v>849</v>
       </c>
       <c r="K151" s="3"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
         <v>106</v>
       </c>
       <c r="D152" t="s">
-        <v>873</v>
+        <v>835</v>
       </c>
       <c r="E152" t="s">
         <v>119</v>
@@ -8617,16 +8617,16 @@
         <v>119</v>
       </c>
       <c r="J152" t="s">
-        <v>891</v>
+        <v>853</v>
       </c>
       <c r="K152" s="3"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>106</v>
       </c>
       <c r="D153" t="s">
-        <v>874</v>
+        <v>836</v>
       </c>
       <c r="E153" t="s">
         <v>119</v>
@@ -8641,16 +8641,16 @@
         <v>119</v>
       </c>
       <c r="J153" t="s">
-        <v>893</v>
+        <v>855</v>
       </c>
       <c r="K153" s="3"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>106</v>
       </c>
       <c r="D154" t="s">
-        <v>875</v>
+        <v>837</v>
       </c>
       <c r="E154" t="s">
         <v>119</v>
@@ -8665,19 +8665,19 @@
         <v>119</v>
       </c>
       <c r="J154" t="s">
-        <v>890</v>
+        <v>852</v>
       </c>
       <c r="K154" s="3"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>881</v>
+        <v>843</v>
       </c>
       <c r="B155" t="s">
         <v>106</v>
       </c>
       <c r="D155" t="s">
-        <v>876</v>
+        <v>838</v>
       </c>
       <c r="E155" t="s">
         <v>119</v>
@@ -8692,19 +8692,19 @@
         <v>119</v>
       </c>
       <c r="J155" t="s">
-        <v>886</v>
+        <v>848</v>
       </c>
       <c r="K155" s="3"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>882</v>
+        <v>844</v>
       </c>
       <c r="B156" t="s">
         <v>106</v>
       </c>
       <c r="D156" t="s">
-        <v>877</v>
+        <v>839</v>
       </c>
       <c r="E156" t="s">
         <v>119</v>
@@ -8719,16 +8719,16 @@
         <v>119</v>
       </c>
       <c r="J156" t="s">
-        <v>888</v>
+        <v>850</v>
       </c>
       <c r="K156" s="3"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>106</v>
       </c>
       <c r="D157" t="s">
-        <v>878</v>
+        <v>840</v>
       </c>
       <c r="E157" t="s">
         <v>119</v>
@@ -8743,16 +8743,16 @@
         <v>119</v>
       </c>
       <c r="J157" t="s">
-        <v>892</v>
+        <v>854</v>
       </c>
       <c r="K157" s="3"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
         <v>106</v>
       </c>
       <c r="D158" t="s">
-        <v>879</v>
+        <v>841</v>
       </c>
       <c r="E158" t="s">
         <v>119</v>
@@ -8767,11 +8767,11 @@
         <v>119</v>
       </c>
       <c r="J158" t="s">
-        <v>894</v>
+        <v>856</v>
       </c>
       <c r="K158" s="3"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>273</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>316</v>
       </c>
@@ -8823,7 +8823,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>246</v>
       </c>
@@ -8846,10 +8846,10 @@
         <v>119</v>
       </c>
       <c r="J161" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>441</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>443</v>
       </c>
@@ -8901,7 +8901,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>439</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>445</v>
       </c>
@@ -8953,7 +8953,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>442</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>444</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>440</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>446</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>437</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>438</v>
       </c>
@@ -9109,7 +9109,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>505</v>
       </c>
@@ -9135,7 +9135,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>510</v>
       </c>
@@ -9161,7 +9161,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>275</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>345</v>
       </c>
@@ -9213,7 +9213,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>275</v>
       </c>
@@ -9239,7 +9239,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>484</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>353</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>354</v>
       </c>
@@ -9317,7 +9317,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>317</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>456</v>
       </c>
@@ -9369,7 +9369,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>487</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>404</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>363</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>405</v>
       </c>
@@ -9499,7 +9499,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>364</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>403</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>400</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>401</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>512</v>
       </c>
@@ -9629,7 +9629,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>511</v>
       </c>
@@ -9655,7 +9655,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>450</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>451</v>
       </c>
@@ -9707,7 +9707,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>369</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>370</v>
       </c>
@@ -9759,7 +9759,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>368</v>
       </c>
@@ -9785,7 +9785,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>499</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>583</v>
       </c>
@@ -9837,7 +9837,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>584</v>
       </c>
@@ -9863,7 +9863,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>501</v>
       </c>
@@ -9889,7 +9889,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>502</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>500</v>
       </c>
@@ -9941,15 +9941,15 @@
         <v>496</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>906</v>
+        <v>868</v>
       </c>
       <c r="B204" t="s">
         <v>106</v>
       </c>
       <c r="D204" t="s">
-        <v>904</v>
+        <v>866</v>
       </c>
       <c r="E204" t="s">
         <v>153</v>
@@ -9964,18 +9964,18 @@
         <v>119</v>
       </c>
       <c r="J204" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>907</v>
+        <v>869</v>
       </c>
       <c r="B205" t="s">
         <v>106</v>
       </c>
       <c r="D205" t="s">
-        <v>905</v>
+        <v>867</v>
       </c>
       <c r="E205" t="s">
         <v>153</v>
@@ -9990,10 +9990,10 @@
         <v>119</v>
       </c>
       <c r="J205" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>285</v>
       </c>
@@ -10019,15 +10019,15 @@
         <v>302</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>830</v>
+        <v>928</v>
       </c>
       <c r="B207" t="s">
         <v>106</v>
       </c>
       <c r="D207" t="s">
-        <v>831</v>
+        <v>914</v>
       </c>
       <c r="E207" t="s">
         <v>119</v>
@@ -10045,15 +10045,15 @@
         <v>597</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>832</v>
+        <v>929</v>
       </c>
       <c r="B208" t="s">
         <v>106</v>
       </c>
       <c r="D208" t="s">
-        <v>833</v>
+        <v>915</v>
       </c>
       <c r="E208" t="s">
         <v>119</v>
@@ -10071,15 +10071,15 @@
         <v>301</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>834</v>
+        <v>930</v>
       </c>
       <c r="B209" t="s">
         <v>106</v>
       </c>
       <c r="D209" t="s">
-        <v>835</v>
+        <v>916</v>
       </c>
       <c r="E209" t="s">
         <v>119</v>
@@ -10097,15 +10097,15 @@
         <v>599</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>836</v>
+        <v>931</v>
       </c>
       <c r="B210" t="s">
         <v>106</v>
       </c>
       <c r="D210" t="s">
-        <v>837</v>
+        <v>917</v>
       </c>
       <c r="E210" t="s">
         <v>119</v>
@@ -10123,15 +10123,15 @@
         <v>598</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>838</v>
+        <v>932</v>
       </c>
       <c r="B211" t="s">
         <v>106</v>
       </c>
       <c r="D211" t="s">
-        <v>839</v>
+        <v>918</v>
       </c>
       <c r="E211" t="s">
         <v>153</v>
@@ -10149,15 +10149,15 @@
         <v>601</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>840</v>
+        <v>933</v>
       </c>
       <c r="B212" t="s">
         <v>106</v>
       </c>
       <c r="D212" t="s">
-        <v>841</v>
+        <v>919</v>
       </c>
       <c r="E212" t="s">
         <v>153</v>
@@ -10172,18 +10172,18 @@
         <v>119</v>
       </c>
       <c r="J212" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>843</v>
+        <v>947</v>
       </c>
       <c r="B213" t="s">
         <v>106</v>
       </c>
       <c r="D213" t="s">
-        <v>844</v>
+        <v>946</v>
       </c>
       <c r="E213" t="s">
         <v>153</v>
@@ -10198,18 +10198,18 @@
         <v>119</v>
       </c>
       <c r="J213" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>848</v>
+        <v>934</v>
       </c>
       <c r="B214" t="s">
         <v>106</v>
       </c>
       <c r="D214" t="s">
-        <v>847</v>
+        <v>920</v>
       </c>
       <c r="E214" t="s">
         <v>153</v>
@@ -10224,18 +10224,18 @@
         <v>119</v>
       </c>
       <c r="J214" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>815</v>
+        <v>935</v>
       </c>
       <c r="B215" t="s">
         <v>106</v>
       </c>
       <c r="D215" t="s">
-        <v>812</v>
+        <v>921</v>
       </c>
       <c r="E215" t="s">
         <v>119</v>
@@ -10253,15 +10253,15 @@
         <v>597</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>816</v>
+        <v>936</v>
       </c>
       <c r="B216" t="s">
         <v>106</v>
       </c>
       <c r="D216" t="s">
-        <v>811</v>
+        <v>922</v>
       </c>
       <c r="E216" t="s">
         <v>119</v>
@@ -10279,15 +10279,15 @@
         <v>301</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>820</v>
+        <v>937</v>
       </c>
       <c r="B217" t="s">
         <v>106</v>
       </c>
       <c r="D217" t="s">
-        <v>813</v>
+        <v>923</v>
       </c>
       <c r="E217" t="s">
         <v>119</v>
@@ -10305,15 +10305,15 @@
         <v>599</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>817</v>
+        <v>938</v>
       </c>
       <c r="B218" t="s">
         <v>106</v>
       </c>
       <c r="D218" t="s">
-        <v>814</v>
+        <v>924</v>
       </c>
       <c r="E218" t="s">
         <v>119</v>
@@ -10331,15 +10331,15 @@
         <v>598</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>818</v>
+        <v>939</v>
       </c>
       <c r="B219" t="s">
         <v>106</v>
       </c>
       <c r="D219" t="s">
-        <v>810</v>
+        <v>925</v>
       </c>
       <c r="E219" t="s">
         <v>153</v>
@@ -10357,15 +10357,15 @@
         <v>601</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>819</v>
+        <v>940</v>
       </c>
       <c r="B220" t="s">
         <v>106</v>
       </c>
       <c r="D220" t="s">
-        <v>809</v>
+        <v>926</v>
       </c>
       <c r="E220" t="s">
         <v>153</v>
@@ -10383,15 +10383,15 @@
         <v>600</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>826</v>
+        <v>948</v>
       </c>
       <c r="B221" t="s">
         <v>106</v>
       </c>
       <c r="D221" t="s">
-        <v>821</v>
+        <v>942</v>
       </c>
       <c r="E221" t="s">
         <v>153</v>
@@ -10406,18 +10406,18 @@
         <v>119</v>
       </c>
       <c r="J221" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>827</v>
+        <v>949</v>
       </c>
       <c r="B222" t="s">
         <v>106</v>
       </c>
       <c r="D222" t="s">
-        <v>822</v>
+        <v>943</v>
       </c>
       <c r="E222" t="s">
         <v>153</v>
@@ -10435,15 +10435,15 @@
         <v>304</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>829</v>
+        <v>950</v>
       </c>
       <c r="B223" t="s">
         <v>106</v>
       </c>
       <c r="D223" t="s">
-        <v>823</v>
+        <v>944</v>
       </c>
       <c r="E223" t="s">
         <v>153</v>
@@ -10461,15 +10461,15 @@
         <v>304</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>828</v>
+        <v>951</v>
       </c>
       <c r="B224" t="s">
         <v>106</v>
       </c>
       <c r="D224" t="s">
-        <v>824</v>
+        <v>945</v>
       </c>
       <c r="E224" t="s">
         <v>153</v>
@@ -10487,15 +10487,15 @@
         <v>304</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>849</v>
+        <v>941</v>
       </c>
       <c r="B225" t="s">
         <v>106</v>
       </c>
       <c r="D225" t="s">
-        <v>846</v>
+        <v>927</v>
       </c>
       <c r="E225" t="s">
         <v>153</v>
@@ -10510,18 +10510,18 @@
         <v>119</v>
       </c>
       <c r="J225" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>901</v>
+        <v>863</v>
       </c>
       <c r="B226" t="s">
         <v>106</v>
       </c>
       <c r="D226" t="s">
-        <v>895</v>
+        <v>857</v>
       </c>
       <c r="E226" t="s">
         <v>153</v>
@@ -10536,18 +10536,18 @@
         <v>119</v>
       </c>
       <c r="J226" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>902</v>
+        <v>864</v>
       </c>
       <c r="B227" t="s">
         <v>106</v>
       </c>
       <c r="D227" t="s">
-        <v>896</v>
+        <v>858</v>
       </c>
       <c r="E227" t="s">
         <v>153</v>
@@ -10562,18 +10562,18 @@
         <v>119</v>
       </c>
       <c r="J227" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>903</v>
+        <v>865</v>
       </c>
       <c r="B228" t="s">
         <v>106</v>
       </c>
       <c r="D228" t="s">
-        <v>897</v>
+        <v>859</v>
       </c>
       <c r="E228" t="s">
         <v>153</v>
@@ -10588,18 +10588,18 @@
         <v>119</v>
       </c>
       <c r="J228" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>857</v>
+        <v>819</v>
       </c>
       <c r="B229" t="s">
         <v>106</v>
       </c>
       <c r="D229" t="s">
-        <v>852</v>
+        <v>814</v>
       </c>
       <c r="E229" t="s">
         <v>153</v>
@@ -10614,18 +10614,18 @@
         <v>119</v>
       </c>
       <c r="J229" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>858</v>
+        <v>820</v>
       </c>
       <c r="B230" t="s">
         <v>106</v>
       </c>
       <c r="D230" t="s">
-        <v>853</v>
+        <v>815</v>
       </c>
       <c r="E230" t="s">
         <v>153</v>
@@ -10640,18 +10640,18 @@
         <v>119</v>
       </c>
       <c r="J230" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>859</v>
+        <v>821</v>
       </c>
       <c r="B231" t="s">
         <v>106</v>
       </c>
       <c r="D231" t="s">
-        <v>854</v>
+        <v>816</v>
       </c>
       <c r="E231" t="s">
         <v>153</v>
@@ -10666,18 +10666,18 @@
         <v>119</v>
       </c>
       <c r="J231" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>860</v>
+        <v>822</v>
       </c>
       <c r="B232" t="s">
         <v>106</v>
       </c>
       <c r="D232" t="s">
-        <v>855</v>
+        <v>817</v>
       </c>
       <c r="E232" t="s">
         <v>153</v>
@@ -10692,18 +10692,18 @@
         <v>119</v>
       </c>
       <c r="J232" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>861</v>
+        <v>823</v>
       </c>
       <c r="B233" t="s">
         <v>106</v>
       </c>
       <c r="D233" t="s">
-        <v>856</v>
+        <v>818</v>
       </c>
       <c r="E233" t="s">
         <v>153</v>
@@ -10718,10 +10718,10 @@
         <v>119</v>
       </c>
       <c r="J233" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>341</v>
       </c>
@@ -10747,7 +10747,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>561</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>562</v>
       </c>
@@ -10799,7 +10799,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>560</v>
       </c>
@@ -10825,7 +10825,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>468</v>
       </c>
@@ -10851,7 +10851,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>469</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>470</v>
       </c>
@@ -10903,7 +10903,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>471</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>619</v>
       </c>
@@ -10955,7 +10955,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>620</v>
       </c>
@@ -10981,7 +10981,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>623</v>
       </c>
@@ -11007,7 +11007,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>622</v>
       </c>
@@ -11033,7 +11033,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>621</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>624</v>
       </c>
@@ -11085,7 +11085,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>625</v>
       </c>
@@ -11111,7 +11111,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>626</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>627</v>
       </c>
@@ -11163,7 +11163,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>628</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>629</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>630</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>631</v>
       </c>
@@ -11267,7 +11267,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>632</v>
       </c>
@@ -11293,7 +11293,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>633</v>
       </c>
@@ -11319,7 +11319,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>634</v>
       </c>
@@ -11345,7 +11345,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>635</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>636</v>
       </c>
@@ -11397,7 +11397,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>637</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>638</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>639</v>
       </c>
@@ -11475,7 +11475,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>640</v>
       </c>
@@ -11501,7 +11501,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>641</v>
       </c>
@@ -11527,7 +11527,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>642</v>
       </c>
@@ -11553,7 +11553,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>643</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>644</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>645</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>646</v>
       </c>
@@ -11657,7 +11657,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>647</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>648</v>
       </c>
@@ -11709,7 +11709,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>649</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>650</v>
       </c>
@@ -11761,7 +11761,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>651</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>652</v>
       </c>
@@ -11813,7 +11813,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>654</v>
       </c>
@@ -11839,7 +11839,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>653</v>
       </c>
@@ -11865,7 +11865,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>655</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>656</v>
       </c>
@@ -11917,15 +11917,15 @@
         <v>707</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>867</v>
+        <v>829</v>
       </c>
       <c r="B280" t="s">
         <v>602</v>
       </c>
       <c r="D280" t="s">
-        <v>868</v>
+        <v>830</v>
       </c>
       <c r="E280" t="s">
         <v>153</v>
@@ -11940,10 +11940,10 @@
         <v>119</v>
       </c>
       <c r="J280" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>702</v>
       </c>
@@ -11969,7 +11969,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>703</v>
       </c>
@@ -11995,7 +11995,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>657</v>
       </c>
@@ -12021,7 +12021,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>658</v>
       </c>
@@ -12047,7 +12047,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>270</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>271</v>
       </c>
@@ -12099,7 +12099,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>272</v>
       </c>
@@ -12125,7 +12125,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>81</v>
       </c>
@@ -12149,7 +12149,7 @@
       </c>
       <c r="K288" s="3"/>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>40</v>
       </c>
@@ -12175,7 +12175,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>72</v>
       </c>
@@ -12198,7 +12198,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>39</v>
       </c>
@@ -12224,7 +12224,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>69</v>
       </c>
@@ -12250,7 +12250,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>170</v>
       </c>
@@ -12273,7 +12273,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>178</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>187</v>
       </c>
@@ -12313,7 +12313,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>71</v>
       </c>
@@ -12333,7 +12333,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>70</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>76</v>
       </c>
@@ -12373,7 +12373,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>75</v>
       </c>
@@ -12393,7 +12393,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>74</v>
       </c>
@@ -12413,7 +12413,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>88</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>89</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>50</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>188</v>
       </c>
@@ -12493,7 +12493,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>177</v>
       </c>
@@ -12513,7 +12513,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>26</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>95</v>
       </c>
@@ -12553,7 +12553,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>94</v>
       </c>
@@ -12573,7 +12573,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>97</v>
       </c>
@@ -12593,7 +12593,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>96</v>
       </c>
@@ -12613,7 +12613,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>10</v>
       </c>
@@ -12633,7 +12633,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>84</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>83</v>
       </c>
@@ -12673,7 +12673,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>38</v>
       </c>
@@ -12699,7 +12699,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>183</v>
       </c>
@@ -12725,7 +12725,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>263</v>
       </c>
@@ -12751,7 +12751,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>17</v>
       </c>
@@ -12777,7 +12777,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>260</v>
       </c>
@@ -12804,7 +12804,7 @@
       </c>
       <c r="K318" s="3"/>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>262</v>
       </c>
@@ -12830,7 +12830,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>261</v>
       </c>
@@ -12856,7 +12856,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>264</v>
       </c>
@@ -12882,7 +12882,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>115</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>184</v>
       </c>
@@ -12931,7 +12931,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>18</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>19</v>
       </c>
@@ -12977,7 +12977,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>133</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>14</v>
       </c>
@@ -13017,7 +13017,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>15</v>
       </c>
@@ -13037,7 +13037,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>4</v>
       </c>
@@ -13057,7 +13057,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>20</v>
       </c>
@@ -13077,7 +13077,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>31</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>27</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>550</v>
       </c>
@@ -13143,7 +13143,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>165</v>
       </c>
@@ -13166,7 +13166,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>93</v>
       </c>
@@ -13189,7 +13189,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>91</v>
       </c>
@@ -13212,7 +13212,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>90</v>
       </c>
@@ -13235,26 +13235,26 @@
         <v>186</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>945</v>
+        <v>907</v>
       </c>
       <c r="B338" t="s">
         <v>106</v>
       </c>
       <c r="D338" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>947</v>
+        <v>909</v>
       </c>
       <c r="B339" t="s">
         <v>106</v>
       </c>
       <c r="D339" t="s">
-        <v>948</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added variable to variable list
</commit_message>
<xml_diff>
--- a/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
+++ b/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccaradon\Documents\GitHub\ComStock\measures\comstock_sensitivity_reports\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aallen\Documents\GitHub\comstock_new_branch\ComStock\measures\comstock_sensitivity_reports\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942F525B-C61E-4E32-BD07-233845842D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1816A07A-B17A-4A34-829C-9791585B7052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="672" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3028" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="963">
   <si>
     <t>Input List</t>
   </si>
@@ -2923,6 +2923,12 @@
   </si>
   <si>
     <t>com_report_hvac_count_water_water_heat_pumps_cooling</t>
+  </si>
+  <si>
+    <t>Average airflow ratio for VAV systems</t>
+  </si>
+  <si>
+    <t>air_system_vav_avg_flow_ratio</t>
   </si>
 </sst>
 </file>
@@ -4737,11 +4743,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE568D5-2279-4922-8B77-550F2E5B90B6}">
-  <dimension ref="A1:K343"/>
+  <dimension ref="A1:K344"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D213" sqref="D213"/>
+      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I344" sqref="I344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13386,13 +13392,36 @@
         <v>928</v>
       </c>
     </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>961</v>
+      </c>
+      <c r="B344" t="s">
+        <v>106</v>
+      </c>
+      <c r="D344" t="s">
+        <v>962</v>
+      </c>
+      <c r="E344" t="s">
+        <v>152</v>
+      </c>
+      <c r="F344" t="s">
+        <v>141</v>
+      </c>
+      <c r="H344" t="s">
+        <v>119</v>
+      </c>
+      <c r="I344" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K341" xr:uid="{723ACE23-DD34-4680-B6C8-8AA325E563AF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K341">
       <sortCondition ref="B1:B341"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="E2:E341 H2:I341 J16:J21 J86:J91 J105 J117 J149 J214">
+  <conditionalFormatting sqref="E2:E341 H2:I341 J16:J21 J86:J91 J105 J117 J149 J214 E344">
     <cfRule type="containsText" dxfId="9" priority="38" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E2)))</formula>
     </cfRule>
@@ -13400,7 +13429,7 @@
       <formula>NOT(ISERROR(SEARCH("yes",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E341">
+  <conditionalFormatting sqref="E2:E341 E344">
     <cfRule type="containsText" dxfId="7" priority="35" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
adding outputs to variable list
</commit_message>
<xml_diff>
--- a/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
+++ b/measures/comstock_sensitivity_reports/resources/Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccaradon\Documents\GitHub\ComStock\measures\comstock_sensitivity_reports\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aallen\Documents\GitHub\comstock_new_branch\ComStock\measures\comstock_sensitivity_reports\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942F525B-C61E-4E32-BD07-233845842D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF8D4F7-3708-4E24-921D-CB6B622C9CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="672" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{35549412-5E91-4CB3-A95B-F037AB4A5442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3028" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3052" uniqueCount="970">
   <si>
     <t>Input List</t>
   </si>
@@ -2923,6 +2923,33 @@
   </si>
   <si>
     <t>com_report_hvac_count_water_water_heat_pumps_cooling</t>
+  </si>
+  <si>
+    <t>com_stock_sensitivity_reports.has_htg_setback_all_tstats</t>
+  </si>
+  <si>
+    <t>com_stock_sensitivity_reports.has_clg_setback_all_tstats</t>
+  </si>
+  <si>
+    <t>com_stock_sensitivity_reports.at_least_one_htg_setback</t>
+  </si>
+  <si>
+    <t>com_stock_sensitivity_reports.at_least_one_clg_setback</t>
+  </si>
+  <si>
+    <t>Has heating setbacks in all thermostats</t>
+  </si>
+  <si>
+    <t>Has cooling setbacks in all thermostats</t>
+  </si>
+  <si>
+    <t>Has at least one zone with a heating setback</t>
+  </si>
+  <si>
+    <t>Has at least one zone with a cooling setback</t>
+  </si>
+  <si>
+    <t>to_string</t>
   </si>
 </sst>
 </file>
@@ -4737,16 +4764,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE568D5-2279-4922-8B77-550F2E5B90B6}">
-  <dimension ref="A1:K343"/>
+  <dimension ref="A1:K347"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D213" sqref="D213"/>
+      <pane ySplit="1" topLeftCell="A314" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I344" sqref="I344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="70.85546875" bestFit="1" customWidth="1"/>
@@ -13386,13 +13413,93 @@
         <v>928</v>
       </c>
     </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>965</v>
+      </c>
+      <c r="B344" t="s">
+        <v>106</v>
+      </c>
+      <c r="D344" t="s">
+        <v>961</v>
+      </c>
+      <c r="E344" t="s">
+        <v>152</v>
+      </c>
+      <c r="F344" t="s">
+        <v>969</v>
+      </c>
+      <c r="H344" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>966</v>
+      </c>
+      <c r="B345" t="s">
+        <v>106</v>
+      </c>
+      <c r="D345" t="s">
+        <v>962</v>
+      </c>
+      <c r="E345" t="s">
+        <v>152</v>
+      </c>
+      <c r="F345" t="s">
+        <v>969</v>
+      </c>
+      <c r="H345" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>967</v>
+      </c>
+      <c r="B346" t="s">
+        <v>106</v>
+      </c>
+      <c r="D346" t="s">
+        <v>963</v>
+      </c>
+      <c r="E346" t="s">
+        <v>152</v>
+      </c>
+      <c r="F346" t="s">
+        <v>969</v>
+      </c>
+      <c r="H346" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>968</v>
+      </c>
+      <c r="B347" t="s">
+        <v>106</v>
+      </c>
+      <c r="D347" t="s">
+        <v>964</v>
+      </c>
+      <c r="E347" t="s">
+        <v>152</v>
+      </c>
+      <c r="F347" t="s">
+        <v>969</v>
+      </c>
+      <c r="H347" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K341" xr:uid="{723ACE23-DD34-4680-B6C8-8AA325E563AF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K341">
       <sortCondition ref="B1:B341"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="E2:E341 H2:I341 J16:J21 J86:J91 J105 J117 J149 J214">
+  <conditionalFormatting sqref="E2:E341 H2:I341 J16:J21 J86:J91 J105 J117 J149 J214 E344:F347">
     <cfRule type="containsText" dxfId="9" priority="38" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E2)))</formula>
     </cfRule>
@@ -13400,7 +13507,7 @@
       <formula>NOT(ISERROR(SEARCH("yes",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E341">
+  <conditionalFormatting sqref="E2:E341 E344:F347">
     <cfRule type="containsText" dxfId="7" priority="35" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E2)))</formula>
     </cfRule>

</xml_diff>